<commit_message>
fancy defense scoring rd1
</commit_message>
<xml_diff>
--- a/points.xlsx
+++ b/points.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nshnipes\Documents\git\Fantasy_Football\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7312CFF7-D22A-4D8F-98A0-8CC7AA7282D6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C1FD9B-EB6D-409E-BAD5-BAD015AE815D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{662825C1-5B8B-46F7-8367-88E39E477269}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="126">
   <si>
     <t>punting</t>
   </si>
@@ -409,13 +409,16 @@
   </si>
   <si>
     <t>yds</t>
+  </si>
+  <si>
+    <t>third_down_stop_failed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -428,6 +431,12 @@
       <color rgb="FF000000"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -450,57 +459,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -810,10 +779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D1EE4CB-20AA-4C42-AD2C-6DDD49B959EF}">
-  <dimension ref="A1:D111"/>
+  <dimension ref="A1:D112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D103" sqref="A1:D103"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2125,6 +2094,20 @@
       </c>
       <c r="D111" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>23</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C112">
+        <v>-0.1</v>
+      </c>
+      <c r="D112" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>